<commit_message>
edit protocol and data sheets
</commit_message>
<xml_diff>
--- a/data/song_measurements_2017.xlsx
+++ b/data/song_measurements_2017.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -513,7 +514,7 @@
   <dimension ref="A1:AF13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -882,6 +883,39 @@
       <c r="E11" t="s">
         <v>41</v>
       </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+      <c r="K11">
+        <v>5</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>2</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="Z11">
+        <v>1</v>
+      </c>
+      <c r="AA11">
+        <v>1</v>
+      </c>
+      <c r="AB11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -893,6 +927,30 @@
       <c r="E12" t="s">
         <v>41</v>
       </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>5</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>2</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -903,6 +961,39 @@
       </c>
       <c r="E13" t="s">
         <v>41</v>
+      </c>
+      <c r="J13">
+        <v>3</v>
+      </c>
+      <c r="K13">
+        <v>5</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+      <c r="Z13">
+        <v>1</v>
+      </c>
+      <c r="AA13">
+        <v>1</v>
+      </c>
+      <c r="AB13">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>